<commit_message>
Added Interceptors To Decentralize Logic
</commit_message>
<xml_diff>
--- a/DataTypesWorkbook.xlsx
+++ b/DataTypesWorkbook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Fourth Of July</t>
+  </si>
+  <si>
+    <t>UniqueId</t>
+  </si>
+  <si>
+    <t>A23B58EC-8BB3-413F-BBBE-CCE71E470594</t>
+  </si>
+  <si>
+    <t>6C5B3800-B097-4C52-85ED-A92321FCC9B0</t>
   </si>
 </sst>
 </file>
@@ -367,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -378,7 +387,7 @@
     <col min="1" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +403,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -412,8 +424,11 @@
         <f>((1/52)/5)*B2</f>
         <v>7.6923076923076927E-3</v>
       </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -429,6 +444,9 @@
       <c r="E3">
         <f>((1/52)/5)*B3</f>
         <v>3.8461538461538464E-3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V3.1 solving Decimal Parse error
</commit_message>
<xml_diff>
--- a/DataTypesWorkbook.xlsx
+++ b/DataTypesWorkbook.xlsx
@@ -379,7 +379,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -439,7 +439,7 @@
         <v>42189</v>
       </c>
       <c r="D3" s="2">
-        <v>100</v>
+        <v>1.4999999999999901E-2</v>
       </c>
       <c r="E3">
         <f>((1/52)/5)*B3</f>

</xml_diff>